<commit_message>
New version on levelCreator.xlsx
</commit_message>
<xml_diff>
--- a/FarthorlPacMan/DataFiles/levelCreator.xlsx
+++ b/FarthorlPacMan/DataFiles/levelCreator.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saiva\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyan.ivanov\Desktop\FarthorlPacMan\trunk\FarthorlPacMan\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="GraphicMatrix" sheetId="1" r:id="rId1"/>
     <sheet name="Matrix - result" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,23 +371,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -423,23 +406,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -594,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,19 +688,19 @@
         <v>0</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>0</v>
@@ -800,19 +766,19 @@
         <v>3</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>3</v>
@@ -1730,7 +1696,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="srW5Qi5SjKEK+HcMoN36gYoYp/0E6gOzEyfVGM7O0GaF8WQ+pv/2C+JGQfxbFZvSbJG6yqN4FbBaxnnK+3P2ug==" saltValue="2FhCcDzrr5Sxp3opMbWX0g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="nT0g/K6+1uzUfh5uAzAqcG8bZuMt+M+UPZH/vKMFYAtiDiYZWdeRjJN3y+eWF0ZvLNnPBMOazF7yXrnkgFxafw==" saltValue="wtT3OpfVdqQ8zjmElFvwVA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="B2:Y14">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"1"</formula>
@@ -1744,6 +1710,11 @@
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B2:Y14">
+      <formula1>"0,1"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1754,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="A20" sqref="A1:C1048576"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,7 +1748,7 @@
         <v>0,1</v>
       </c>
       <c r="D1" s="13" t="str">
-        <f>A1&amp;","&amp;B1&amp;"="&amp;C1</f>
+        <f t="shared" ref="D1:D64" si="0">A1&amp;","&amp;B1&amp;"="&amp;C1</f>
         <v>0,0=0,1</v>
       </c>
     </row>
@@ -1793,7 +1764,7 @@
         <v>0,1</v>
       </c>
       <c r="D2" s="13" t="str">
-        <f>A2&amp;","&amp;B2&amp;"="&amp;C2</f>
+        <f t="shared" si="0"/>
         <v>0,1=0,1</v>
       </c>
     </row>
@@ -1809,7 +1780,7 @@
         <v>0,1</v>
       </c>
       <c r="D3" s="13" t="str">
-        <f>A3&amp;","&amp;B3&amp;"="&amp;C3</f>
+        <f t="shared" si="0"/>
         <v>0,2=0,1</v>
       </c>
     </row>
@@ -1825,7 +1796,7 @@
         <v>0,1</v>
       </c>
       <c r="D4" s="13" t="str">
-        <f>A4&amp;","&amp;B4&amp;"="&amp;C4</f>
+        <f t="shared" si="0"/>
         <v>0,3=0,1</v>
       </c>
     </row>
@@ -1841,7 +1812,7 @@
         <v>0,1</v>
       </c>
       <c r="D5" s="13" t="str">
-        <f>A5&amp;","&amp;B5&amp;"="&amp;C5</f>
+        <f t="shared" si="0"/>
         <v>0,4=0,1</v>
       </c>
     </row>
@@ -1857,7 +1828,7 @@
         <v>0,1</v>
       </c>
       <c r="D6" s="13" t="str">
-        <f>A6&amp;","&amp;B6&amp;"="&amp;C6</f>
+        <f t="shared" si="0"/>
         <v>0,5=0,1</v>
       </c>
     </row>
@@ -1873,7 +1844,7 @@
         <v>0,1</v>
       </c>
       <c r="D7" s="13" t="str">
-        <f>A7&amp;","&amp;B7&amp;"="&amp;C7</f>
+        <f t="shared" si="0"/>
         <v>0,6=0,1</v>
       </c>
     </row>
@@ -1889,7 +1860,7 @@
         <v>0,1</v>
       </c>
       <c r="D8" s="13" t="str">
-        <f>A8&amp;","&amp;B8&amp;"="&amp;C8</f>
+        <f t="shared" si="0"/>
         <v>0,7=0,1</v>
       </c>
     </row>
@@ -1905,7 +1876,7 @@
         <v>0,1</v>
       </c>
       <c r="D9" s="13" t="str">
-        <f>A9&amp;","&amp;B9&amp;"="&amp;C9</f>
+        <f t="shared" si="0"/>
         <v>0,8=0,1</v>
       </c>
     </row>
@@ -1921,7 +1892,7 @@
         <v>0,1</v>
       </c>
       <c r="D10" s="13" t="str">
-        <f>A10&amp;","&amp;B10&amp;"="&amp;C10</f>
+        <f t="shared" si="0"/>
         <v>0,9=0,1</v>
       </c>
     </row>
@@ -1937,7 +1908,7 @@
         <v>0,1</v>
       </c>
       <c r="D11" s="13" t="str">
-        <f>A11&amp;","&amp;B11&amp;"="&amp;C11</f>
+        <f t="shared" si="0"/>
         <v>0,10=0,1</v>
       </c>
     </row>
@@ -1953,7 +1924,7 @@
         <v>0,1</v>
       </c>
       <c r="D12" s="13" t="str">
-        <f>A12&amp;","&amp;B12&amp;"="&amp;C12</f>
+        <f t="shared" si="0"/>
         <v>0,11=0,1</v>
       </c>
     </row>
@@ -1969,7 +1940,7 @@
         <v>0,1</v>
       </c>
       <c r="D13" s="13" t="str">
-        <f>A13&amp;","&amp;B13&amp;"="&amp;C13</f>
+        <f t="shared" si="0"/>
         <v>0,12=0,1</v>
       </c>
     </row>
@@ -1985,7 +1956,7 @@
         <v>0,1</v>
       </c>
       <c r="D14" s="13" t="str">
-        <f>A14&amp;","&amp;B14&amp;"="&amp;C14</f>
+        <f t="shared" si="0"/>
         <v>1,0=0,1</v>
       </c>
     </row>
@@ -2001,7 +1972,7 @@
         <v>1,0</v>
       </c>
       <c r="D15" s="13" t="str">
-        <f>A15&amp;","&amp;B15&amp;"="&amp;C15</f>
+        <f t="shared" si="0"/>
         <v>1,1=1,0</v>
       </c>
     </row>
@@ -2017,7 +1988,7 @@
         <v>0,1</v>
       </c>
       <c r="D16" s="13" t="str">
-        <f>A16&amp;","&amp;B16&amp;"="&amp;C16</f>
+        <f t="shared" si="0"/>
         <v>1,2=0,1</v>
       </c>
     </row>
@@ -2033,7 +2004,7 @@
         <v>0,1</v>
       </c>
       <c r="D17" s="13" t="str">
-        <f>A17&amp;","&amp;B17&amp;"="&amp;C17</f>
+        <f t="shared" si="0"/>
         <v>1,3=0,1</v>
       </c>
     </row>
@@ -2049,7 +2020,7 @@
         <v>0,1</v>
       </c>
       <c r="D18" s="13" t="str">
-        <f>A18&amp;","&amp;B18&amp;"="&amp;C18</f>
+        <f t="shared" si="0"/>
         <v>1,4=0,1</v>
       </c>
     </row>
@@ -2065,7 +2036,7 @@
         <v>1,0</v>
       </c>
       <c r="D19" s="13" t="str">
-        <f>A19&amp;","&amp;B19&amp;"="&amp;C19</f>
+        <f t="shared" si="0"/>
         <v>1,5=1,0</v>
       </c>
     </row>
@@ -2081,7 +2052,7 @@
         <v>1,0</v>
       </c>
       <c r="D20" s="13" t="str">
-        <f>A20&amp;","&amp;B20&amp;"="&amp;C20</f>
+        <f t="shared" si="0"/>
         <v>1,6=1,0</v>
       </c>
     </row>
@@ -2097,7 +2068,7 @@
         <v>1,0</v>
       </c>
       <c r="D21" s="13" t="str">
-        <f>A21&amp;","&amp;B21&amp;"="&amp;C21</f>
+        <f t="shared" si="0"/>
         <v>1,7=1,0</v>
       </c>
     </row>
@@ -2113,7 +2084,7 @@
         <v>0,1</v>
       </c>
       <c r="D22" s="13" t="str">
-        <f>A22&amp;","&amp;B22&amp;"="&amp;C22</f>
+        <f t="shared" si="0"/>
         <v>1,8=0,1</v>
       </c>
     </row>
@@ -2129,7 +2100,7 @@
         <v>1,0</v>
       </c>
       <c r="D23" s="13" t="str">
-        <f>A23&amp;","&amp;B23&amp;"="&amp;C23</f>
+        <f t="shared" si="0"/>
         <v>1,9=1,0</v>
       </c>
     </row>
@@ -2145,7 +2116,7 @@
         <v>0,1</v>
       </c>
       <c r="D24" s="13" t="str">
-        <f>A24&amp;","&amp;B24&amp;"="&amp;C24</f>
+        <f t="shared" si="0"/>
         <v>1,10=0,1</v>
       </c>
     </row>
@@ -2161,7 +2132,7 @@
         <v>1,0</v>
       </c>
       <c r="D25" s="13" t="str">
-        <f>A25&amp;","&amp;B25&amp;"="&amp;C25</f>
+        <f t="shared" si="0"/>
         <v>1,11=1,0</v>
       </c>
     </row>
@@ -2177,7 +2148,7 @@
         <v>0,1</v>
       </c>
       <c r="D26" s="13" t="str">
-        <f>A26&amp;","&amp;B26&amp;"="&amp;C26</f>
+        <f t="shared" si="0"/>
         <v>1,12=0,1</v>
       </c>
     </row>
@@ -2193,7 +2164,7 @@
         <v>0,1</v>
       </c>
       <c r="D27" s="13" t="str">
-        <f>A27&amp;","&amp;B27&amp;"="&amp;C27</f>
+        <f t="shared" si="0"/>
         <v>2,0=0,1</v>
       </c>
     </row>
@@ -2209,7 +2180,7 @@
         <v>1,0</v>
       </c>
       <c r="D28" s="13" t="str">
-        <f>A28&amp;","&amp;B28&amp;"="&amp;C28</f>
+        <f t="shared" si="0"/>
         <v>2,1=1,0</v>
       </c>
     </row>
@@ -2225,7 +2196,7 @@
         <v>0,1</v>
       </c>
       <c r="D29" s="13" t="str">
-        <f>A29&amp;","&amp;B29&amp;"="&amp;C29</f>
+        <f t="shared" si="0"/>
         <v>2,2=0,1</v>
       </c>
     </row>
@@ -2241,7 +2212,7 @@
         <v>0,1</v>
       </c>
       <c r="D30" s="13" t="str">
-        <f>A30&amp;","&amp;B30&amp;"="&amp;C30</f>
+        <f t="shared" si="0"/>
         <v>2,3=0,1</v>
       </c>
     </row>
@@ -2257,7 +2228,7 @@
         <v>0,1</v>
       </c>
       <c r="D31" s="13" t="str">
-        <f>A31&amp;","&amp;B31&amp;"="&amp;C31</f>
+        <f t="shared" si="0"/>
         <v>2,4=0,1</v>
       </c>
     </row>
@@ -2273,7 +2244,7 @@
         <v>1,0</v>
       </c>
       <c r="D32" s="13" t="str">
-        <f>A32&amp;","&amp;B32&amp;"="&amp;C32</f>
+        <f t="shared" si="0"/>
         <v>2,5=1,0</v>
       </c>
     </row>
@@ -2289,7 +2260,7 @@
         <v>0,1</v>
       </c>
       <c r="D33" s="13" t="str">
-        <f>A33&amp;","&amp;B33&amp;"="&amp;C33</f>
+        <f t="shared" si="0"/>
         <v>2,6=0,1</v>
       </c>
     </row>
@@ -2305,7 +2276,7 @@
         <v>0,1</v>
       </c>
       <c r="D34" s="13" t="str">
-        <f>A34&amp;","&amp;B34&amp;"="&amp;C34</f>
+        <f t="shared" si="0"/>
         <v>2,7=0,1</v>
       </c>
     </row>
@@ -2321,7 +2292,7 @@
         <v>0,1</v>
       </c>
       <c r="D35" s="13" t="str">
-        <f>A35&amp;","&amp;B35&amp;"="&amp;C35</f>
+        <f t="shared" si="0"/>
         <v>2,8=0,1</v>
       </c>
     </row>
@@ -2337,7 +2308,7 @@
         <v>1,0</v>
       </c>
       <c r="D36" s="13" t="str">
-        <f>A36&amp;","&amp;B36&amp;"="&amp;C36</f>
+        <f t="shared" si="0"/>
         <v>2,9=1,0</v>
       </c>
     </row>
@@ -2353,7 +2324,7 @@
         <v>0,1</v>
       </c>
       <c r="D37" s="13" t="str">
-        <f>A37&amp;","&amp;B37&amp;"="&amp;C37</f>
+        <f t="shared" si="0"/>
         <v>2,10=0,1</v>
       </c>
     </row>
@@ -2369,7 +2340,7 @@
         <v>0,1</v>
       </c>
       <c r="D38" s="13" t="str">
-        <f>A38&amp;","&amp;B38&amp;"="&amp;C38</f>
+        <f t="shared" si="0"/>
         <v>2,11=0,1</v>
       </c>
     </row>
@@ -2385,7 +2356,7 @@
         <v>0,1</v>
       </c>
       <c r="D39" s="13" t="str">
-        <f>A39&amp;","&amp;B39&amp;"="&amp;C39</f>
+        <f t="shared" si="0"/>
         <v>2,12=0,1</v>
       </c>
     </row>
@@ -2401,7 +2372,7 @@
         <v>0,1</v>
       </c>
       <c r="D40" s="13" t="str">
-        <f>A40&amp;","&amp;B40&amp;"="&amp;C40</f>
+        <f t="shared" si="0"/>
         <v>3,0=0,1</v>
       </c>
     </row>
@@ -2417,7 +2388,7 @@
         <v>1,0</v>
       </c>
       <c r="D41" s="13" t="str">
-        <f>A41&amp;","&amp;B41&amp;"="&amp;C41</f>
+        <f t="shared" si="0"/>
         <v>3,1=1,0</v>
       </c>
     </row>
@@ -2433,7 +2404,7 @@
         <v>1,0</v>
       </c>
       <c r="D42" s="13" t="str">
-        <f>A42&amp;","&amp;B42&amp;"="&amp;C42</f>
+        <f t="shared" si="0"/>
         <v>3,2=1,0</v>
       </c>
     </row>
@@ -2449,7 +2420,7 @@
         <v>1,0</v>
       </c>
       <c r="D43" s="13" t="str">
-        <f>A43&amp;","&amp;B43&amp;"="&amp;C43</f>
+        <f t="shared" si="0"/>
         <v>3,3=1,0</v>
       </c>
     </row>
@@ -2465,7 +2436,7 @@
         <v>0,1</v>
       </c>
       <c r="D44" s="13" t="str">
-        <f>A44&amp;","&amp;B44&amp;"="&amp;C44</f>
+        <f t="shared" si="0"/>
         <v>3,4=0,1</v>
       </c>
     </row>
@@ -2481,7 +2452,7 @@
         <v>1,0</v>
       </c>
       <c r="D45" s="13" t="str">
-        <f>A45&amp;","&amp;B45&amp;"="&amp;C45</f>
+        <f t="shared" si="0"/>
         <v>3,5=1,0</v>
       </c>
     </row>
@@ -2497,7 +2468,7 @@
         <v>0,1</v>
       </c>
       <c r="D46" s="13" t="str">
-        <f>A46&amp;","&amp;B46&amp;"="&amp;C46</f>
+        <f t="shared" si="0"/>
         <v>3,6=0,1</v>
       </c>
     </row>
@@ -2513,7 +2484,7 @@
         <v>1,0</v>
       </c>
       <c r="D47" s="13" t="str">
-        <f>A47&amp;","&amp;B47&amp;"="&amp;C47</f>
+        <f t="shared" si="0"/>
         <v>3,7=1,0</v>
       </c>
     </row>
@@ -2529,7 +2500,7 @@
         <v>0,1</v>
       </c>
       <c r="D48" s="13" t="str">
-        <f>A48&amp;","&amp;B48&amp;"="&amp;C48</f>
+        <f t="shared" si="0"/>
         <v>3,8=0,1</v>
       </c>
     </row>
@@ -2545,7 +2516,7 @@
         <v>1,0</v>
       </c>
       <c r="D49" s="13" t="str">
-        <f>A49&amp;","&amp;B49&amp;"="&amp;C49</f>
+        <f t="shared" si="0"/>
         <v>3,9=1,0</v>
       </c>
     </row>
@@ -2561,7 +2532,7 @@
         <v>1,0</v>
       </c>
       <c r="D50" s="13" t="str">
-        <f>A50&amp;","&amp;B50&amp;"="&amp;C50</f>
+        <f t="shared" si="0"/>
         <v>3,10=1,0</v>
       </c>
     </row>
@@ -2577,7 +2548,7 @@
         <v>1,0</v>
       </c>
       <c r="D51" s="13" t="str">
-        <f>A51&amp;","&amp;B51&amp;"="&amp;C51</f>
+        <f t="shared" si="0"/>
         <v>3,11=1,0</v>
       </c>
     </row>
@@ -2593,7 +2564,7 @@
         <v>0,1</v>
       </c>
       <c r="D52" s="13" t="str">
-        <f>A52&amp;","&amp;B52&amp;"="&amp;C52</f>
+        <f t="shared" si="0"/>
         <v>3,12=0,1</v>
       </c>
     </row>
@@ -2609,7 +2580,7 @@
         <v>0,1</v>
       </c>
       <c r="D53" s="13" t="str">
-        <f>A53&amp;","&amp;B53&amp;"="&amp;C53</f>
+        <f t="shared" si="0"/>
         <v>4,0=0,1</v>
       </c>
     </row>
@@ -2625,7 +2596,7 @@
         <v>0,1</v>
       </c>
       <c r="D54" s="13" t="str">
-        <f>A54&amp;","&amp;B54&amp;"="&amp;C54</f>
+        <f t="shared" si="0"/>
         <v>4,1=0,1</v>
       </c>
     </row>
@@ -2641,7 +2612,7 @@
         <v>0,1</v>
       </c>
       <c r="D55" s="13" t="str">
-        <f>A55&amp;","&amp;B55&amp;"="&amp;C55</f>
+        <f t="shared" si="0"/>
         <v>4,2=0,1</v>
       </c>
     </row>
@@ -2657,7 +2628,7 @@
         <v>0,1</v>
       </c>
       <c r="D56" s="13" t="str">
-        <f>A56&amp;","&amp;B56&amp;"="&amp;C56</f>
+        <f t="shared" si="0"/>
         <v>4,3=0,1</v>
       </c>
     </row>
@@ -2673,7 +2644,7 @@
         <v>0,1</v>
       </c>
       <c r="D57" s="13" t="str">
-        <f>A57&amp;","&amp;B57&amp;"="&amp;C57</f>
+        <f t="shared" si="0"/>
         <v>4,4=0,1</v>
       </c>
     </row>
@@ -2689,7 +2660,7 @@
         <v>0,1</v>
       </c>
       <c r="D58" s="13" t="str">
-        <f>A58&amp;","&amp;B58&amp;"="&amp;C58</f>
+        <f t="shared" si="0"/>
         <v>4,5=0,1</v>
       </c>
     </row>
@@ -2705,7 +2676,7 @@
         <v>0,1</v>
       </c>
       <c r="D59" s="13" t="str">
-        <f>A59&amp;","&amp;B59&amp;"="&amp;C59</f>
+        <f t="shared" si="0"/>
         <v>4,6=0,1</v>
       </c>
     </row>
@@ -2721,7 +2692,7 @@
         <v>1,0</v>
       </c>
       <c r="D60" s="13" t="str">
-        <f>A60&amp;","&amp;B60&amp;"="&amp;C60</f>
+        <f t="shared" si="0"/>
         <v>4,7=1,0</v>
       </c>
     </row>
@@ -2737,7 +2708,7 @@
         <v>0,1</v>
       </c>
       <c r="D61" s="13" t="str">
-        <f>A61&amp;","&amp;B61&amp;"="&amp;C61</f>
+        <f t="shared" si="0"/>
         <v>4,8=0,1</v>
       </c>
     </row>
@@ -2753,7 +2724,7 @@
         <v>0,1</v>
       </c>
       <c r="D62" s="13" t="str">
-        <f>A62&amp;","&amp;B62&amp;"="&amp;C62</f>
+        <f t="shared" si="0"/>
         <v>4,9=0,1</v>
       </c>
     </row>
@@ -2769,7 +2740,7 @@
         <v>0,1</v>
       </c>
       <c r="D63" s="13" t="str">
-        <f>A63&amp;","&amp;B63&amp;"="&amp;C63</f>
+        <f t="shared" si="0"/>
         <v>4,10=0,1</v>
       </c>
     </row>
@@ -2785,7 +2756,7 @@
         <v>0,1</v>
       </c>
       <c r="D64" s="13" t="str">
-        <f>A64&amp;","&amp;B64&amp;"="&amp;C64</f>
+        <f t="shared" si="0"/>
         <v>4,11=0,1</v>
       </c>
     </row>
@@ -2801,7 +2772,7 @@
         <v>0,1</v>
       </c>
       <c r="D65" s="13" t="str">
-        <f>A65&amp;","&amp;B65&amp;"="&amp;C65</f>
+        <f t="shared" ref="D65:D128" si="1">A65&amp;","&amp;B65&amp;"="&amp;C65</f>
         <v>4,12=0,1</v>
       </c>
     </row>
@@ -2817,7 +2788,7 @@
         <v>0,1</v>
       </c>
       <c r="D66" s="13" t="str">
-        <f>A66&amp;","&amp;B66&amp;"="&amp;C66</f>
+        <f t="shared" si="1"/>
         <v>5,0=0,1</v>
       </c>
     </row>
@@ -2833,7 +2804,7 @@
         <v>1,0</v>
       </c>
       <c r="D67" s="13" t="str">
-        <f>A67&amp;","&amp;B67&amp;"="&amp;C67</f>
+        <f t="shared" si="1"/>
         <v>5,1=1,0</v>
       </c>
     </row>
@@ -2849,7 +2820,7 @@
         <v>1,0</v>
       </c>
       <c r="D68" s="13" t="str">
-        <f>A68&amp;","&amp;B68&amp;"="&amp;C68</f>
+        <f t="shared" si="1"/>
         <v>5,2=1,0</v>
       </c>
     </row>
@@ -2865,7 +2836,7 @@
         <v>1,0</v>
       </c>
       <c r="D69" s="13" t="str">
-        <f>A69&amp;","&amp;B69&amp;"="&amp;C69</f>
+        <f t="shared" si="1"/>
         <v>5,3=1,0</v>
       </c>
     </row>
@@ -2881,7 +2852,7 @@
         <v>1,0</v>
       </c>
       <c r="D70" s="13" t="str">
-        <f>A70&amp;","&amp;B70&amp;"="&amp;C70</f>
+        <f t="shared" si="1"/>
         <v>5,4=1,0</v>
       </c>
     </row>
@@ -2897,7 +2868,7 @@
         <v>1,0</v>
       </c>
       <c r="D71" s="13" t="str">
-        <f>A71&amp;","&amp;B71&amp;"="&amp;C71</f>
+        <f t="shared" si="1"/>
         <v>5,5=1,0</v>
       </c>
     </row>
@@ -2913,7 +2884,7 @@
         <v>0,1</v>
       </c>
       <c r="D72" s="13" t="str">
-        <f>A72&amp;","&amp;B72&amp;"="&amp;C72</f>
+        <f t="shared" si="1"/>
         <v>5,6=0,1</v>
       </c>
     </row>
@@ -2929,7 +2900,7 @@
         <v>1,0</v>
       </c>
       <c r="D73" s="13" t="str">
-        <f>A73&amp;","&amp;B73&amp;"="&amp;C73</f>
+        <f t="shared" si="1"/>
         <v>5,7=1,0</v>
       </c>
     </row>
@@ -2945,7 +2916,7 @@
         <v>1,0</v>
       </c>
       <c r="D74" s="13" t="str">
-        <f>A74&amp;","&amp;B74&amp;"="&amp;C74</f>
+        <f t="shared" si="1"/>
         <v>5,8=1,0</v>
       </c>
     </row>
@@ -2961,7 +2932,7 @@
         <v>1,0</v>
       </c>
       <c r="D75" s="13" t="str">
-        <f>A75&amp;","&amp;B75&amp;"="&amp;C75</f>
+        <f t="shared" si="1"/>
         <v>5,9=1,0</v>
       </c>
     </row>
@@ -2977,7 +2948,7 @@
         <v>1,0</v>
       </c>
       <c r="D76" s="13" t="str">
-        <f>A76&amp;","&amp;B76&amp;"="&amp;C76</f>
+        <f t="shared" si="1"/>
         <v>5,10=1,0</v>
       </c>
     </row>
@@ -2993,7 +2964,7 @@
         <v>1,0</v>
       </c>
       <c r="D77" s="13" t="str">
-        <f>A77&amp;","&amp;B77&amp;"="&amp;C77</f>
+        <f t="shared" si="1"/>
         <v>5,11=1,0</v>
       </c>
     </row>
@@ -3009,7 +2980,7 @@
         <v>1,0</v>
       </c>
       <c r="D78" s="13" t="str">
-        <f>A78&amp;","&amp;B78&amp;"="&amp;C78</f>
+        <f t="shared" si="1"/>
         <v>5,12=1,0</v>
       </c>
     </row>
@@ -3025,7 +2996,7 @@
         <v>0,1</v>
       </c>
       <c r="D79" s="13" t="str">
-        <f>A79&amp;","&amp;B79&amp;"="&amp;C79</f>
+        <f t="shared" si="1"/>
         <v>6,0=0,1</v>
       </c>
     </row>
@@ -3041,7 +3012,7 @@
         <v>0,1</v>
       </c>
       <c r="D80" s="13" t="str">
-        <f>A80&amp;","&amp;B80&amp;"="&amp;C80</f>
+        <f t="shared" si="1"/>
         <v>6,1=0,1</v>
       </c>
     </row>
@@ -3057,7 +3028,7 @@
         <v>0,1</v>
       </c>
       <c r="D81" s="13" t="str">
-        <f>A81&amp;","&amp;B81&amp;"="&amp;C81</f>
+        <f t="shared" si="1"/>
         <v>6,2=0,1</v>
       </c>
     </row>
@@ -3073,7 +3044,7 @@
         <v>0,1</v>
       </c>
       <c r="D82" s="13" t="str">
-        <f>A82&amp;","&amp;B82&amp;"="&amp;C82</f>
+        <f t="shared" si="1"/>
         <v>6,3=0,1</v>
       </c>
     </row>
@@ -3089,7 +3060,7 @@
         <v>0,1</v>
       </c>
       <c r="D83" s="13" t="str">
-        <f>A83&amp;","&amp;B83&amp;"="&amp;C83</f>
+        <f t="shared" si="1"/>
         <v>6,4=0,1</v>
       </c>
     </row>
@@ -3105,7 +3076,7 @@
         <v>0,1</v>
       </c>
       <c r="D84" s="13" t="str">
-        <f>A84&amp;","&amp;B84&amp;"="&amp;C84</f>
+        <f t="shared" si="1"/>
         <v>6,5=0,1</v>
       </c>
     </row>
@@ -3121,7 +3092,7 @@
         <v>0,1</v>
       </c>
       <c r="D85" s="13" t="str">
-        <f>A85&amp;","&amp;B85&amp;"="&amp;C85</f>
+        <f t="shared" si="1"/>
         <v>6,6=0,1</v>
       </c>
     </row>
@@ -3137,7 +3108,7 @@
         <v>0,1</v>
       </c>
       <c r="D86" s="13" t="str">
-        <f>A86&amp;","&amp;B86&amp;"="&amp;C86</f>
+        <f t="shared" si="1"/>
         <v>6,7=0,1</v>
       </c>
     </row>
@@ -3153,7 +3124,7 @@
         <v>0,1</v>
       </c>
       <c r="D87" s="13" t="str">
-        <f>A87&amp;","&amp;B87&amp;"="&amp;C87</f>
+        <f t="shared" si="1"/>
         <v>6,8=0,1</v>
       </c>
     </row>
@@ -3169,7 +3140,7 @@
         <v>0,1</v>
       </c>
       <c r="D88" s="13" t="str">
-        <f>A88&amp;","&amp;B88&amp;"="&amp;C88</f>
+        <f t="shared" si="1"/>
         <v>6,9=0,1</v>
       </c>
     </row>
@@ -3185,7 +3156,7 @@
         <v>0,1</v>
       </c>
       <c r="D89" s="13" t="str">
-        <f>A89&amp;","&amp;B89&amp;"="&amp;C89</f>
+        <f t="shared" si="1"/>
         <v>6,10=0,1</v>
       </c>
     </row>
@@ -3201,7 +3172,7 @@
         <v>0,1</v>
       </c>
       <c r="D90" s="13" t="str">
-        <f>A90&amp;","&amp;B90&amp;"="&amp;C90</f>
+        <f t="shared" si="1"/>
         <v>6,11=0,1</v>
       </c>
     </row>
@@ -3217,7 +3188,7 @@
         <v>0,1</v>
       </c>
       <c r="D91" s="13" t="str">
-        <f>A91&amp;","&amp;B91&amp;"="&amp;C91</f>
+        <f t="shared" si="1"/>
         <v>6,12=0,1</v>
       </c>
     </row>
@@ -3233,7 +3204,7 @@
         <v>1,0</v>
       </c>
       <c r="D92" s="13" t="str">
-        <f>A92&amp;","&amp;B92&amp;"="&amp;C92</f>
+        <f t="shared" si="1"/>
         <v>7,0=1,0</v>
       </c>
     </row>
@@ -3249,7 +3220,7 @@
         <v>1,0</v>
       </c>
       <c r="D93" s="13" t="str">
-        <f>A93&amp;","&amp;B93&amp;"="&amp;C93</f>
+        <f t="shared" si="1"/>
         <v>7,1=1,0</v>
       </c>
     </row>
@@ -3265,7 +3236,7 @@
         <v>1,0</v>
       </c>
       <c r="D94" s="13" t="str">
-        <f>A94&amp;","&amp;B94&amp;"="&amp;C94</f>
+        <f t="shared" si="1"/>
         <v>7,2=1,0</v>
       </c>
     </row>
@@ -3281,7 +3252,7 @@
         <v>1,0</v>
       </c>
       <c r="D95" s="13" t="str">
-        <f>A95&amp;","&amp;B95&amp;"="&amp;C95</f>
+        <f t="shared" si="1"/>
         <v>7,3=1,0</v>
       </c>
     </row>
@@ -3297,7 +3268,7 @@
         <v>0,1</v>
       </c>
       <c r="D96" s="13" t="str">
-        <f>A96&amp;","&amp;B96&amp;"="&amp;C96</f>
+        <f t="shared" si="1"/>
         <v>7,4=0,1</v>
       </c>
     </row>
@@ -3313,7 +3284,7 @@
         <v>1,0</v>
       </c>
       <c r="D97" s="13" t="str">
-        <f>A97&amp;","&amp;B97&amp;"="&amp;C97</f>
+        <f t="shared" si="1"/>
         <v>7,5=1,0</v>
       </c>
     </row>
@@ -3329,7 +3300,7 @@
         <v>0,1</v>
       </c>
       <c r="D98" s="13" t="str">
-        <f>A98&amp;","&amp;B98&amp;"="&amp;C98</f>
+        <f t="shared" si="1"/>
         <v>7,6=0,1</v>
       </c>
     </row>
@@ -3345,7 +3316,7 @@
         <v>1,0</v>
       </c>
       <c r="D99" s="13" t="str">
-        <f>A99&amp;","&amp;B99&amp;"="&amp;C99</f>
+        <f t="shared" si="1"/>
         <v>7,7=1,0</v>
       </c>
     </row>
@@ -3361,7 +3332,7 @@
         <v>1,0</v>
       </c>
       <c r="D100" s="13" t="str">
-        <f>A100&amp;","&amp;B100&amp;"="&amp;C100</f>
+        <f t="shared" si="1"/>
         <v>7,8=1,0</v>
       </c>
     </row>
@@ -3377,7 +3348,7 @@
         <v>1,0</v>
       </c>
       <c r="D101" s="13" t="str">
-        <f>A101&amp;","&amp;B101&amp;"="&amp;C101</f>
+        <f t="shared" si="1"/>
         <v>7,9=1,0</v>
       </c>
     </row>
@@ -3393,7 +3364,7 @@
         <v>1,0</v>
       </c>
       <c r="D102" s="13" t="str">
-        <f>A102&amp;","&amp;B102&amp;"="&amp;C102</f>
+        <f t="shared" si="1"/>
         <v>7,10=1,0</v>
       </c>
     </row>
@@ -3409,7 +3380,7 @@
         <v>1,0</v>
       </c>
       <c r="D103" s="13" t="str">
-        <f>A103&amp;","&amp;B103&amp;"="&amp;C103</f>
+        <f t="shared" si="1"/>
         <v>7,11=1,0</v>
       </c>
     </row>
@@ -3425,7 +3396,7 @@
         <v>0,1</v>
       </c>
       <c r="D104" s="13" t="str">
-        <f>A104&amp;","&amp;B104&amp;"="&amp;C104</f>
+        <f t="shared" si="1"/>
         <v>7,12=0,1</v>
       </c>
     </row>
@@ -3441,7 +3412,7 @@
         <v>0,1</v>
       </c>
       <c r="D105" s="13" t="str">
-        <f>A105&amp;","&amp;B105&amp;"="&amp;C105</f>
+        <f t="shared" si="1"/>
         <v>8,0=0,1</v>
       </c>
     </row>
@@ -3457,7 +3428,7 @@
         <v>0,1</v>
       </c>
       <c r="D106" s="13" t="str">
-        <f>A106&amp;","&amp;B106&amp;"="&amp;C106</f>
+        <f t="shared" si="1"/>
         <v>8,1=0,1</v>
       </c>
     </row>
@@ -3473,7 +3444,7 @@
         <v>0,1</v>
       </c>
       <c r="D107" s="13" t="str">
-        <f>A107&amp;","&amp;B107&amp;"="&amp;C107</f>
+        <f t="shared" si="1"/>
         <v>8,2=0,1</v>
       </c>
     </row>
@@ -3489,7 +3460,7 @@
         <v>1,0</v>
       </c>
       <c r="D108" s="13" t="str">
-        <f>A108&amp;","&amp;B108&amp;"="&amp;C108</f>
+        <f t="shared" si="1"/>
         <v>8,3=1,0</v>
       </c>
     </row>
@@ -3505,7 +3476,7 @@
         <v>0,1</v>
       </c>
       <c r="D109" s="13" t="str">
-        <f>A109&amp;","&amp;B109&amp;"="&amp;C109</f>
+        <f t="shared" si="1"/>
         <v>8,4=0,1</v>
       </c>
     </row>
@@ -3521,7 +3492,7 @@
         <v>1,0</v>
       </c>
       <c r="D110" s="13" t="str">
-        <f>A110&amp;","&amp;B110&amp;"="&amp;C110</f>
+        <f t="shared" si="1"/>
         <v>8,5=1,0</v>
       </c>
     </row>
@@ -3537,7 +3508,7 @@
         <v>0,1</v>
       </c>
       <c r="D111" s="13" t="str">
-        <f>A111&amp;","&amp;B111&amp;"="&amp;C111</f>
+        <f t="shared" si="1"/>
         <v>8,6=0,1</v>
       </c>
     </row>
@@ -3553,7 +3524,7 @@
         <v>0,1</v>
       </c>
       <c r="D112" s="13" t="str">
-        <f>A112&amp;","&amp;B112&amp;"="&amp;C112</f>
+        <f t="shared" si="1"/>
         <v>8,7=0,1</v>
       </c>
     </row>
@@ -3569,7 +3540,7 @@
         <v>0,1</v>
       </c>
       <c r="D113" s="13" t="str">
-        <f>A113&amp;","&amp;B113&amp;"="&amp;C113</f>
+        <f t="shared" si="1"/>
         <v>8,8=0,1</v>
       </c>
     </row>
@@ -3585,7 +3556,7 @@
         <v>0,1</v>
       </c>
       <c r="D114" s="13" t="str">
-        <f>A114&amp;","&amp;B114&amp;"="&amp;C114</f>
+        <f t="shared" si="1"/>
         <v>8,9=0,1</v>
       </c>
     </row>
@@ -3601,7 +3572,7 @@
         <v>0,1</v>
       </c>
       <c r="D115" s="13" t="str">
-        <f>A115&amp;","&amp;B115&amp;"="&amp;C115</f>
+        <f t="shared" si="1"/>
         <v>8,10=0,1</v>
       </c>
     </row>
@@ -3617,7 +3588,7 @@
         <v>0,1</v>
       </c>
       <c r="D116" s="13" t="str">
-        <f>A116&amp;","&amp;B116&amp;"="&amp;C116</f>
+        <f t="shared" si="1"/>
         <v>8,11=0,1</v>
       </c>
     </row>
@@ -3633,7 +3604,7 @@
         <v>0,1</v>
       </c>
       <c r="D117" s="13" t="str">
-        <f>A117&amp;","&amp;B117&amp;"="&amp;C117</f>
+        <f t="shared" si="1"/>
         <v>8,12=0,1</v>
       </c>
     </row>
@@ -3649,7 +3620,7 @@
         <v>1,0</v>
       </c>
       <c r="D118" s="13" t="str">
-        <f>A118&amp;","&amp;B118&amp;"="&amp;C118</f>
+        <f t="shared" si="1"/>
         <v>9,0=1,0</v>
       </c>
     </row>
@@ -3665,7 +3636,7 @@
         <v>1,0</v>
       </c>
       <c r="D119" s="13" t="str">
-        <f>A119&amp;","&amp;B119&amp;"="&amp;C119</f>
+        <f t="shared" si="1"/>
         <v>9,1=1,0</v>
       </c>
     </row>
@@ -3681,7 +3652,7 @@
         <v>0,1</v>
       </c>
       <c r="D120" s="13" t="str">
-        <f>A120&amp;","&amp;B120&amp;"="&amp;C120</f>
+        <f t="shared" si="1"/>
         <v>9,2=0,1</v>
       </c>
     </row>
@@ -3697,7 +3668,7 @@
         <v>0,1</v>
       </c>
       <c r="D121" s="13" t="str">
-        <f>A121&amp;","&amp;B121&amp;"="&amp;C121</f>
+        <f t="shared" si="1"/>
         <v>9,3=0,1</v>
       </c>
     </row>
@@ -3713,7 +3684,7 @@
         <v>0,1</v>
       </c>
       <c r="D122" s="13" t="str">
-        <f>A122&amp;","&amp;B122&amp;"="&amp;C122</f>
+        <f t="shared" si="1"/>
         <v>9,4=0,1</v>
       </c>
     </row>
@@ -3729,7 +3700,7 @@
         <v>1,0</v>
       </c>
       <c r="D123" s="13" t="str">
-        <f>A123&amp;","&amp;B123&amp;"="&amp;C123</f>
+        <f t="shared" si="1"/>
         <v>9,5=1,0</v>
       </c>
     </row>
@@ -3745,7 +3716,7 @@
         <v>0,1</v>
       </c>
       <c r="D124" s="13" t="str">
-        <f>A124&amp;","&amp;B124&amp;"="&amp;C124</f>
+        <f t="shared" si="1"/>
         <v>9,6=0,1</v>
       </c>
     </row>
@@ -3761,7 +3732,7 @@
         <v>1,0</v>
       </c>
       <c r="D125" s="13" t="str">
-        <f>A125&amp;","&amp;B125&amp;"="&amp;C125</f>
+        <f t="shared" si="1"/>
         <v>9,7=1,0</v>
       </c>
     </row>
@@ -3777,7 +3748,7 @@
         <v>1,0</v>
       </c>
       <c r="D126" s="13" t="str">
-        <f>A126&amp;","&amp;B126&amp;"="&amp;C126</f>
+        <f t="shared" si="1"/>
         <v>9,8=1,0</v>
       </c>
     </row>
@@ -3793,7 +3764,7 @@
         <v>1,0</v>
       </c>
       <c r="D127" s="13" t="str">
-        <f>A127&amp;","&amp;B127&amp;"="&amp;C127</f>
+        <f t="shared" si="1"/>
         <v>9,9=1,0</v>
       </c>
     </row>
@@ -3809,7 +3780,7 @@
         <v>1,0</v>
       </c>
       <c r="D128" s="13" t="str">
-        <f>A128&amp;","&amp;B128&amp;"="&amp;C128</f>
+        <f t="shared" si="1"/>
         <v>9,10=1,0</v>
       </c>
     </row>
@@ -3825,7 +3796,7 @@
         <v>1,0</v>
       </c>
       <c r="D129" s="13" t="str">
-        <f>A129&amp;","&amp;B129&amp;"="&amp;C129</f>
+        <f t="shared" ref="D129:D192" si="2">A129&amp;","&amp;B129&amp;"="&amp;C129</f>
         <v>9,11=1,0</v>
       </c>
     </row>
@@ -3841,7 +3812,7 @@
         <v>0,1</v>
       </c>
       <c r="D130" s="13" t="str">
-        <f>A130&amp;","&amp;B130&amp;"="&amp;C130</f>
+        <f t="shared" si="2"/>
         <v>9,12=0,1</v>
       </c>
     </row>
@@ -3857,7 +3828,7 @@
         <v>0,1</v>
       </c>
       <c r="D131" s="13" t="str">
-        <f>A131&amp;","&amp;B131&amp;"="&amp;C131</f>
+        <f t="shared" si="2"/>
         <v>10,0=0,1</v>
       </c>
     </row>
@@ -3873,7 +3844,7 @@
         <v>1,0</v>
       </c>
       <c r="D132" s="13" t="str">
-        <f>A132&amp;","&amp;B132&amp;"="&amp;C132</f>
+        <f t="shared" si="2"/>
         <v>10,1=1,0</v>
       </c>
     </row>
@@ -3889,7 +3860,7 @@
         <v>0,1</v>
       </c>
       <c r="D133" s="13" t="str">
-        <f>A133&amp;","&amp;B133&amp;"="&amp;C133</f>
+        <f t="shared" si="2"/>
         <v>10,2=0,1</v>
       </c>
     </row>
@@ -3905,7 +3876,7 @@
         <v>1,0</v>
       </c>
       <c r="D134" s="13" t="str">
-        <f>A134&amp;","&amp;B134&amp;"="&amp;C134</f>
+        <f t="shared" si="2"/>
         <v>10,3=1,0</v>
       </c>
     </row>
@@ -3921,7 +3892,7 @@
         <v>1,0</v>
       </c>
       <c r="D135" s="13" t="str">
-        <f>A135&amp;","&amp;B135&amp;"="&amp;C135</f>
+        <f t="shared" si="2"/>
         <v>10,4=1,0</v>
       </c>
     </row>
@@ -3937,7 +3908,7 @@
         <v>1,0</v>
       </c>
       <c r="D136" s="13" t="str">
-        <f>A136&amp;","&amp;B136&amp;"="&amp;C136</f>
+        <f t="shared" si="2"/>
         <v>10,5=1,0</v>
       </c>
     </row>
@@ -3953,7 +3924,7 @@
         <v>0,1</v>
       </c>
       <c r="D137" s="13" t="str">
-        <f>A137&amp;","&amp;B137&amp;"="&amp;C137</f>
+        <f t="shared" si="2"/>
         <v>10,6=0,1</v>
       </c>
     </row>
@@ -3969,7 +3940,7 @@
         <v>0,1</v>
       </c>
       <c r="D138" s="13" t="str">
-        <f>A138&amp;","&amp;B138&amp;"="&amp;C138</f>
+        <f t="shared" si="2"/>
         <v>10,7=0,1</v>
       </c>
     </row>
@@ -3985,7 +3956,7 @@
         <v>0,1</v>
       </c>
       <c r="D139" s="13" t="str">
-        <f>A139&amp;","&amp;B139&amp;"="&amp;C139</f>
+        <f t="shared" si="2"/>
         <v>10,8=0,1</v>
       </c>
     </row>
@@ -4001,7 +3972,7 @@
         <v>0,1</v>
       </c>
       <c r="D140" s="13" t="str">
-        <f>A140&amp;","&amp;B140&amp;"="&amp;C140</f>
+        <f t="shared" si="2"/>
         <v>10,9=0,1</v>
       </c>
     </row>
@@ -4017,7 +3988,7 @@
         <v>0,1</v>
       </c>
       <c r="D141" s="13" t="str">
-        <f>A141&amp;","&amp;B141&amp;"="&amp;C141</f>
+        <f t="shared" si="2"/>
         <v>10,10=0,1</v>
       </c>
     </row>
@@ -4033,7 +4004,7 @@
         <v>0,1</v>
       </c>
       <c r="D142" s="13" t="str">
-        <f>A142&amp;","&amp;B142&amp;"="&amp;C142</f>
+        <f t="shared" si="2"/>
         <v>10,11=0,1</v>
       </c>
     </row>
@@ -4049,7 +4020,7 @@
         <v>0,1</v>
       </c>
       <c r="D143" s="13" t="str">
-        <f>A143&amp;","&amp;B143&amp;"="&amp;C143</f>
+        <f t="shared" si="2"/>
         <v>10,12=0,1</v>
       </c>
     </row>
@@ -4065,7 +4036,7 @@
         <v>0,1</v>
       </c>
       <c r="D144" s="13" t="str">
-        <f>A144&amp;","&amp;B144&amp;"="&amp;C144</f>
+        <f t="shared" si="2"/>
         <v>11,0=0,1</v>
       </c>
     </row>
@@ -4081,7 +4052,7 @@
         <v>1,0</v>
       </c>
       <c r="D145" s="13" t="str">
-        <f>A145&amp;","&amp;B145&amp;"="&amp;C145</f>
+        <f t="shared" si="2"/>
         <v>11,1=1,0</v>
       </c>
     </row>
@@ -4097,7 +4068,7 @@
         <v>0,1</v>
       </c>
       <c r="D146" s="13" t="str">
-        <f>A146&amp;","&amp;B146&amp;"="&amp;C146</f>
+        <f t="shared" si="2"/>
         <v>11,2=0,1</v>
       </c>
     </row>
@@ -4113,7 +4084,7 @@
         <v>0,1</v>
       </c>
       <c r="D147" s="13" t="str">
-        <f>A147&amp;","&amp;B147&amp;"="&amp;C147</f>
+        <f t="shared" si="2"/>
         <v>11,3=0,1</v>
       </c>
     </row>
@@ -4129,7 +4100,7 @@
         <v>0,1</v>
       </c>
       <c r="D148" s="13" t="str">
-        <f>A148&amp;","&amp;B148&amp;"="&amp;C148</f>
+        <f t="shared" si="2"/>
         <v>11,4=0,1</v>
       </c>
     </row>
@@ -4145,7 +4116,7 @@
         <v>0,1</v>
       </c>
       <c r="D149" s="13" t="str">
-        <f>A149&amp;","&amp;B149&amp;"="&amp;C149</f>
+        <f t="shared" si="2"/>
         <v>11,5=0,1</v>
       </c>
     </row>
@@ -4161,7 +4132,7 @@
         <v>0,1</v>
       </c>
       <c r="D150" s="13" t="str">
-        <f>A150&amp;","&amp;B150&amp;"="&amp;C150</f>
+        <f t="shared" si="2"/>
         <v>11,6=0,1</v>
       </c>
     </row>
@@ -4177,7 +4148,7 @@
         <v>1,0</v>
       </c>
       <c r="D151" s="13" t="str">
-        <f>A151&amp;","&amp;B151&amp;"="&amp;C151</f>
+        <f t="shared" si="2"/>
         <v>11,7=1,0</v>
       </c>
     </row>
@@ -4193,7 +4164,7 @@
         <v>1,0</v>
       </c>
       <c r="D152" s="13" t="str">
-        <f>A152&amp;","&amp;B152&amp;"="&amp;C152</f>
+        <f t="shared" si="2"/>
         <v>11,8=1,0</v>
       </c>
     </row>
@@ -4209,7 +4180,7 @@
         <v>1,0</v>
       </c>
       <c r="D153" s="13" t="str">
-        <f>A153&amp;","&amp;B153&amp;"="&amp;C153</f>
+        <f t="shared" si="2"/>
         <v>11,9=1,0</v>
       </c>
     </row>
@@ -4225,7 +4196,7 @@
         <v>1,0</v>
       </c>
       <c r="D154" s="13" t="str">
-        <f>A154&amp;","&amp;B154&amp;"="&amp;C154</f>
+        <f t="shared" si="2"/>
         <v>11,10=1,0</v>
       </c>
     </row>
@@ -4241,7 +4212,7 @@
         <v>1,0</v>
       </c>
       <c r="D155" s="13" t="str">
-        <f>A155&amp;","&amp;B155&amp;"="&amp;C155</f>
+        <f t="shared" si="2"/>
         <v>11,11=1,0</v>
       </c>
     </row>
@@ -4257,7 +4228,7 @@
         <v>0,1</v>
       </c>
       <c r="D156" s="13" t="str">
-        <f>A156&amp;","&amp;B156&amp;"="&amp;C156</f>
+        <f t="shared" si="2"/>
         <v>11,12=0,1</v>
       </c>
     </row>
@@ -4273,7 +4244,7 @@
         <v>0,1</v>
       </c>
       <c r="D157" s="13" t="str">
-        <f>A157&amp;","&amp;B157&amp;"="&amp;C157</f>
+        <f t="shared" si="2"/>
         <v>12,0=0,1</v>
       </c>
     </row>
@@ -4289,7 +4260,7 @@
         <v>1,0</v>
       </c>
       <c r="D158" s="13" t="str">
-        <f>A158&amp;","&amp;B158&amp;"="&amp;C158</f>
+        <f t="shared" si="2"/>
         <v>12,1=1,0</v>
       </c>
     </row>
@@ -4305,7 +4276,7 @@
         <v>1,0</v>
       </c>
       <c r="D159" s="13" t="str">
-        <f>A159&amp;","&amp;B159&amp;"="&amp;C159</f>
+        <f t="shared" si="2"/>
         <v>12,2=1,0</v>
       </c>
     </row>
@@ -4321,7 +4292,7 @@
         <v>1,0</v>
       </c>
       <c r="D160" s="13" t="str">
-        <f>A160&amp;","&amp;B160&amp;"="&amp;C160</f>
+        <f t="shared" si="2"/>
         <v>12,3=1,0</v>
       </c>
     </row>
@@ -4337,7 +4308,7 @@
         <v>0,1</v>
       </c>
       <c r="D161" s="13" t="str">
-        <f>A161&amp;","&amp;B161&amp;"="&amp;C161</f>
+        <f t="shared" si="2"/>
         <v>12,4=0,1</v>
       </c>
     </row>
@@ -4353,7 +4324,7 @@
         <v>1,0</v>
       </c>
       <c r="D162" s="13" t="str">
-        <f>A162&amp;","&amp;B162&amp;"="&amp;C162</f>
+        <f t="shared" si="2"/>
         <v>12,5=1,0</v>
       </c>
     </row>
@@ -4369,7 +4340,7 @@
         <v>0,1</v>
       </c>
       <c r="D163" s="13" t="str">
-        <f>A163&amp;","&amp;B163&amp;"="&amp;C163</f>
+        <f t="shared" si="2"/>
         <v>12,6=0,1</v>
       </c>
     </row>
@@ -4385,7 +4356,7 @@
         <v>0,1</v>
       </c>
       <c r="D164" s="13" t="str">
-        <f>A164&amp;","&amp;B164&amp;"="&amp;C164</f>
+        <f t="shared" si="2"/>
         <v>12,7=0,1</v>
       </c>
     </row>
@@ -4401,7 +4372,7 @@
         <v>0,1</v>
       </c>
       <c r="D165" s="13" t="str">
-        <f>A165&amp;","&amp;B165&amp;"="&amp;C165</f>
+        <f t="shared" si="2"/>
         <v>12,8=0,1</v>
       </c>
     </row>
@@ -4417,7 +4388,7 @@
         <v>0,1</v>
       </c>
       <c r="D166" s="13" t="str">
-        <f>A166&amp;","&amp;B166&amp;"="&amp;C166</f>
+        <f t="shared" si="2"/>
         <v>12,9=0,1</v>
       </c>
     </row>
@@ -4433,7 +4404,7 @@
         <v>0,1</v>
       </c>
       <c r="D167" s="13" t="str">
-        <f>A167&amp;","&amp;B167&amp;"="&amp;C167</f>
+        <f t="shared" si="2"/>
         <v>12,10=0,1</v>
       </c>
     </row>
@@ -4449,7 +4420,7 @@
         <v>0,1</v>
       </c>
       <c r="D168" s="13" t="str">
-        <f>A168&amp;","&amp;B168&amp;"="&amp;C168</f>
+        <f t="shared" si="2"/>
         <v>12,11=0,1</v>
       </c>
     </row>
@@ -4465,7 +4436,7 @@
         <v>0,1</v>
       </c>
       <c r="D169" s="13" t="str">
-        <f>A169&amp;","&amp;B169&amp;"="&amp;C169</f>
+        <f t="shared" si="2"/>
         <v>12,12=0,1</v>
       </c>
     </row>
@@ -4478,11 +4449,11 @@
       </c>
       <c r="C170" s="1" t="str">
         <f>IF(GraphicMatrix!O2="0","0,1",IF(GraphicMatrix!O2="1","1,0",""))</f>
-        <v>0,1</v>
+        <v>1,0</v>
       </c>
       <c r="D170" s="13" t="str">
-        <f>A170&amp;","&amp;B170&amp;"="&amp;C170</f>
-        <v>13,0=0,1</v>
+        <f t="shared" si="2"/>
+        <v>13,0=1,0</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4494,11 +4465,11 @@
       </c>
       <c r="C171" s="1" t="str">
         <f>IF(GraphicMatrix!O3="0","0,1",IF(GraphicMatrix!O3="1","1,0",""))</f>
-        <v>0,1</v>
+        <v>1,0</v>
       </c>
       <c r="D171" s="13" t="str">
-        <f>A171&amp;","&amp;B171&amp;"="&amp;C171</f>
-        <v>13,1=0,1</v>
+        <f t="shared" si="2"/>
+        <v>13,1=1,0</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4513,7 +4484,7 @@
         <v>0,1</v>
       </c>
       <c r="D172" s="13" t="str">
-        <f>A172&amp;","&amp;B172&amp;"="&amp;C172</f>
+        <f t="shared" si="2"/>
         <v>13,2=0,1</v>
       </c>
     </row>
@@ -4529,7 +4500,7 @@
         <v>0,1</v>
       </c>
       <c r="D173" s="13" t="str">
-        <f>A173&amp;","&amp;B173&amp;"="&amp;C173</f>
+        <f t="shared" si="2"/>
         <v>13,3=0,1</v>
       </c>
     </row>
@@ -4545,7 +4516,7 @@
         <v>0,1</v>
       </c>
       <c r="D174" s="13" t="str">
-        <f>A174&amp;","&amp;B174&amp;"="&amp;C174</f>
+        <f t="shared" si="2"/>
         <v>13,4=0,1</v>
       </c>
     </row>
@@ -4561,7 +4532,7 @@
         <v>0,1</v>
       </c>
       <c r="D175" s="13" t="str">
-        <f>A175&amp;","&amp;B175&amp;"="&amp;C175</f>
+        <f t="shared" si="2"/>
         <v>13,5=0,1</v>
       </c>
     </row>
@@ -4577,7 +4548,7 @@
         <v>0,1</v>
       </c>
       <c r="D176" s="13" t="str">
-        <f>A176&amp;","&amp;B176&amp;"="&amp;C176</f>
+        <f t="shared" si="2"/>
         <v>13,6=0,1</v>
       </c>
     </row>
@@ -4593,7 +4564,7 @@
         <v>1,0</v>
       </c>
       <c r="D177" s="13" t="str">
-        <f>A177&amp;","&amp;B177&amp;"="&amp;C177</f>
+        <f t="shared" si="2"/>
         <v>13,7=1,0</v>
       </c>
     </row>
@@ -4609,7 +4580,7 @@
         <v>1,0</v>
       </c>
       <c r="D178" s="13" t="str">
-        <f>A178&amp;","&amp;B178&amp;"="&amp;C178</f>
+        <f t="shared" si="2"/>
         <v>13,8=1,0</v>
       </c>
     </row>
@@ -4625,7 +4596,7 @@
         <v>1,0</v>
       </c>
       <c r="D179" s="13" t="str">
-        <f>A179&amp;","&amp;B179&amp;"="&amp;C179</f>
+        <f t="shared" si="2"/>
         <v>13,9=1,0</v>
       </c>
     </row>
@@ -4641,7 +4612,7 @@
         <v>1,0</v>
       </c>
       <c r="D180" s="13" t="str">
-        <f>A180&amp;","&amp;B180&amp;"="&amp;C180</f>
+        <f t="shared" si="2"/>
         <v>13,10=1,0</v>
       </c>
     </row>
@@ -4657,7 +4628,7 @@
         <v>1,0</v>
       </c>
       <c r="D181" s="13" t="str">
-        <f>A181&amp;","&amp;B181&amp;"="&amp;C181</f>
+        <f t="shared" si="2"/>
         <v>13,11=1,0</v>
       </c>
     </row>
@@ -4673,7 +4644,7 @@
         <v>1,0</v>
       </c>
       <c r="D182" s="13" t="str">
-        <f>A182&amp;","&amp;B182&amp;"="&amp;C182</f>
+        <f t="shared" si="2"/>
         <v>13,12=1,0</v>
       </c>
     </row>
@@ -4689,7 +4660,7 @@
         <v>1,0</v>
       </c>
       <c r="D183" s="13" t="str">
-        <f>A183&amp;","&amp;B183&amp;"="&amp;C183</f>
+        <f t="shared" si="2"/>
         <v>14,0=1,0</v>
       </c>
     </row>
@@ -4705,7 +4676,7 @@
         <v>1,0</v>
       </c>
       <c r="D184" s="13" t="str">
-        <f>A184&amp;","&amp;B184&amp;"="&amp;C184</f>
+        <f t="shared" si="2"/>
         <v>14,1=1,0</v>
       </c>
     </row>
@@ -4721,7 +4692,7 @@
         <v>0,1</v>
       </c>
       <c r="D185" s="13" t="str">
-        <f>A185&amp;","&amp;B185&amp;"="&amp;C185</f>
+        <f t="shared" si="2"/>
         <v>14,2=0,1</v>
       </c>
     </row>
@@ -4737,7 +4708,7 @@
         <v>1,0</v>
       </c>
       <c r="D186" s="13" t="str">
-        <f>A186&amp;","&amp;B186&amp;"="&amp;C186</f>
+        <f t="shared" si="2"/>
         <v>14,3=1,0</v>
       </c>
     </row>
@@ -4753,7 +4724,7 @@
         <v>1,0</v>
       </c>
       <c r="D187" s="13" t="str">
-        <f>A187&amp;","&amp;B187&amp;"="&amp;C187</f>
+        <f t="shared" si="2"/>
         <v>14,4=1,0</v>
       </c>
     </row>
@@ -4769,7 +4740,7 @@
         <v>0,1</v>
       </c>
       <c r="D188" s="13" t="str">
-        <f>A188&amp;","&amp;B188&amp;"="&amp;C188</f>
+        <f t="shared" si="2"/>
         <v>14,5=0,1</v>
       </c>
     </row>
@@ -4785,7 +4756,7 @@
         <v>1,0</v>
       </c>
       <c r="D189" s="13" t="str">
-        <f>A189&amp;","&amp;B189&amp;"="&amp;C189</f>
+        <f t="shared" si="2"/>
         <v>14,6=1,0</v>
       </c>
     </row>
@@ -4801,7 +4772,7 @@
         <v>0,1</v>
       </c>
       <c r="D190" s="13" t="str">
-        <f>A190&amp;","&amp;B190&amp;"="&amp;C190</f>
+        <f t="shared" si="2"/>
         <v>14,7=0,1</v>
       </c>
     </row>
@@ -4817,7 +4788,7 @@
         <v>0,1</v>
       </c>
       <c r="D191" s="13" t="str">
-        <f>A191&amp;","&amp;B191&amp;"="&amp;C191</f>
+        <f t="shared" si="2"/>
         <v>14,8=0,1</v>
       </c>
     </row>
@@ -4833,7 +4804,7 @@
         <v>0,1</v>
       </c>
       <c r="D192" s="13" t="str">
-        <f>A192&amp;","&amp;B192&amp;"="&amp;C192</f>
+        <f t="shared" si="2"/>
         <v>14,9=0,1</v>
       </c>
     </row>
@@ -4849,7 +4820,7 @@
         <v>0,1</v>
       </c>
       <c r="D193" s="13" t="str">
-        <f>A193&amp;","&amp;B193&amp;"="&amp;C193</f>
+        <f t="shared" ref="D193:D256" si="3">A193&amp;","&amp;B193&amp;"="&amp;C193</f>
         <v>14,10=0,1</v>
       </c>
     </row>
@@ -4865,7 +4836,7 @@
         <v>0,1</v>
       </c>
       <c r="D194" s="13" t="str">
-        <f>A194&amp;","&amp;B194&amp;"="&amp;C194</f>
+        <f t="shared" si="3"/>
         <v>14,11=0,1</v>
       </c>
     </row>
@@ -4881,7 +4852,7 @@
         <v>0,1</v>
       </c>
       <c r="D195" s="13" t="str">
-        <f>A195&amp;","&amp;B195&amp;"="&amp;C195</f>
+        <f t="shared" si="3"/>
         <v>14,12=0,1</v>
       </c>
     </row>
@@ -4894,11 +4865,11 @@
       </c>
       <c r="C196" s="1" t="str">
         <f>IF(GraphicMatrix!Q2="0","0,1",IF(GraphicMatrix!Q2="1","1,0",""))</f>
-        <v>0,1</v>
+        <v>1,0</v>
       </c>
       <c r="D196" s="13" t="str">
-        <f>A196&amp;","&amp;B196&amp;"="&amp;C196</f>
-        <v>15,0=0,1</v>
+        <f t="shared" si="3"/>
+        <v>15,0=1,0</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4910,11 +4881,11 @@
       </c>
       <c r="C197" s="1" t="str">
         <f>IF(GraphicMatrix!Q3="0","0,1",IF(GraphicMatrix!Q3="1","1,0",""))</f>
-        <v>0,1</v>
+        <v>1,0</v>
       </c>
       <c r="D197" s="13" t="str">
-        <f>A197&amp;","&amp;B197&amp;"="&amp;C197</f>
-        <v>15,1=0,1</v>
+        <f t="shared" si="3"/>
+        <v>15,1=1,0</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4929,7 +4900,7 @@
         <v>0,1</v>
       </c>
       <c r="D198" s="13" t="str">
-        <f>A198&amp;","&amp;B198&amp;"="&amp;C198</f>
+        <f t="shared" si="3"/>
         <v>15,2=0,1</v>
       </c>
     </row>
@@ -4945,7 +4916,7 @@
         <v>0,1</v>
       </c>
       <c r="D199" s="13" t="str">
-        <f>A199&amp;","&amp;B199&amp;"="&amp;C199</f>
+        <f t="shared" si="3"/>
         <v>15,3=0,1</v>
       </c>
     </row>
@@ -4961,7 +4932,7 @@
         <v>1,0</v>
       </c>
       <c r="D200" s="13" t="str">
-        <f>A200&amp;","&amp;B200&amp;"="&amp;C200</f>
+        <f t="shared" si="3"/>
         <v>15,4=1,0</v>
       </c>
     </row>
@@ -4977,7 +4948,7 @@
         <v>0,1</v>
       </c>
       <c r="D201" s="13" t="str">
-        <f>A201&amp;","&amp;B201&amp;"="&amp;C201</f>
+        <f t="shared" si="3"/>
         <v>15,5=0,1</v>
       </c>
     </row>
@@ -4993,7 +4964,7 @@
         <v>0,1</v>
       </c>
       <c r="D202" s="13" t="str">
-        <f>A202&amp;","&amp;B202&amp;"="&amp;C202</f>
+        <f t="shared" si="3"/>
         <v>15,6=0,1</v>
       </c>
     </row>
@@ -5009,7 +4980,7 @@
         <v>0,1</v>
       </c>
       <c r="D203" s="13" t="str">
-        <f>A203&amp;","&amp;B203&amp;"="&amp;C203</f>
+        <f t="shared" si="3"/>
         <v>15,7=0,1</v>
       </c>
     </row>
@@ -5025,7 +4996,7 @@
         <v>1,0</v>
       </c>
       <c r="D204" s="13" t="str">
-        <f>A204&amp;","&amp;B204&amp;"="&amp;C204</f>
+        <f t="shared" si="3"/>
         <v>15,8=1,0</v>
       </c>
     </row>
@@ -5041,7 +5012,7 @@
         <v>1,0</v>
       </c>
       <c r="D205" s="13" t="str">
-        <f>A205&amp;","&amp;B205&amp;"="&amp;C205</f>
+        <f t="shared" si="3"/>
         <v>15,9=1,0</v>
       </c>
     </row>
@@ -5057,7 +5028,7 @@
         <v>1,0</v>
       </c>
       <c r="D206" s="13" t="str">
-        <f>A206&amp;","&amp;B206&amp;"="&amp;C206</f>
+        <f t="shared" si="3"/>
         <v>15,10=1,0</v>
       </c>
     </row>
@@ -5073,7 +5044,7 @@
         <v>1,0</v>
       </c>
       <c r="D207" s="13" t="str">
-        <f>A207&amp;","&amp;B207&amp;"="&amp;C207</f>
+        <f t="shared" si="3"/>
         <v>15,11=1,0</v>
       </c>
     </row>
@@ -5089,7 +5060,7 @@
         <v>1,0</v>
       </c>
       <c r="D208" s="13" t="str">
-        <f>A208&amp;","&amp;B208&amp;"="&amp;C208</f>
+        <f t="shared" si="3"/>
         <v>15,12=1,0</v>
       </c>
     </row>
@@ -5105,7 +5076,7 @@
         <v>1,0</v>
       </c>
       <c r="D209" s="13" t="str">
-        <f>A209&amp;","&amp;B209&amp;"="&amp;C209</f>
+        <f t="shared" si="3"/>
         <v>16,0=1,0</v>
       </c>
     </row>
@@ -5121,7 +5092,7 @@
         <v>1,0</v>
       </c>
       <c r="D210" s="13" t="str">
-        <f>A210&amp;","&amp;B210&amp;"="&amp;C210</f>
+        <f t="shared" si="3"/>
         <v>16,1=1,0</v>
       </c>
     </row>
@@ -5137,7 +5108,7 @@
         <v>1,0</v>
       </c>
       <c r="D211" s="13" t="str">
-        <f>A211&amp;","&amp;B211&amp;"="&amp;C211</f>
+        <f t="shared" si="3"/>
         <v>16,2=1,0</v>
       </c>
     </row>
@@ -5153,7 +5124,7 @@
         <v>0,1</v>
       </c>
       <c r="D212" s="13" t="str">
-        <f>A212&amp;","&amp;B212&amp;"="&amp;C212</f>
+        <f t="shared" si="3"/>
         <v>16,3=0,1</v>
       </c>
     </row>
@@ -5169,7 +5140,7 @@
         <v>1,0</v>
       </c>
       <c r="D213" s="13" t="str">
-        <f>A213&amp;","&amp;B213&amp;"="&amp;C213</f>
+        <f t="shared" si="3"/>
         <v>16,4=1,0</v>
       </c>
     </row>
@@ -5185,7 +5156,7 @@
         <v>0,1</v>
       </c>
       <c r="D214" s="13" t="str">
-        <f>A214&amp;","&amp;B214&amp;"="&amp;C214</f>
+        <f t="shared" si="3"/>
         <v>16,5=0,1</v>
       </c>
     </row>
@@ -5201,7 +5172,7 @@
         <v>1,0</v>
       </c>
       <c r="D215" s="13" t="str">
-        <f>A215&amp;","&amp;B215&amp;"="&amp;C215</f>
+        <f t="shared" si="3"/>
         <v>16,6=1,0</v>
       </c>
     </row>
@@ -5217,7 +5188,7 @@
         <v>1,0</v>
       </c>
       <c r="D216" s="13" t="str">
-        <f>A216&amp;","&amp;B216&amp;"="&amp;C216</f>
+        <f t="shared" si="3"/>
         <v>16,7=1,0</v>
       </c>
     </row>
@@ -5233,7 +5204,7 @@
         <v>0,1</v>
       </c>
       <c r="D217" s="13" t="str">
-        <f>A217&amp;","&amp;B217&amp;"="&amp;C217</f>
+        <f t="shared" si="3"/>
         <v>16,8=0,1</v>
       </c>
     </row>
@@ -5249,7 +5220,7 @@
         <v>0,1</v>
       </c>
       <c r="D218" s="13" t="str">
-        <f>A218&amp;","&amp;B218&amp;"="&amp;C218</f>
+        <f t="shared" si="3"/>
         <v>16,9=0,1</v>
       </c>
     </row>
@@ -5265,7 +5236,7 @@
         <v>0,1</v>
       </c>
       <c r="D219" s="13" t="str">
-        <f>A219&amp;","&amp;B219&amp;"="&amp;C219</f>
+        <f t="shared" si="3"/>
         <v>16,10=0,1</v>
       </c>
     </row>
@@ -5281,7 +5252,7 @@
         <v>0,1</v>
       </c>
       <c r="D220" s="13" t="str">
-        <f>A220&amp;","&amp;B220&amp;"="&amp;C220</f>
+        <f t="shared" si="3"/>
         <v>16,11=0,1</v>
       </c>
     </row>
@@ -5297,7 +5268,7 @@
         <v>0,1</v>
       </c>
       <c r="D221" s="13" t="str">
-        <f>A221&amp;","&amp;B221&amp;"="&amp;C221</f>
+        <f t="shared" si="3"/>
         <v>16,12=0,1</v>
       </c>
     </row>
@@ -5310,11 +5281,11 @@
       </c>
       <c r="C222" s="1" t="str">
         <f>IF(GraphicMatrix!S2="0","0,1",IF(GraphicMatrix!S2="1","1,0",""))</f>
-        <v>0,1</v>
+        <v>1,0</v>
       </c>
       <c r="D222" s="13" t="str">
-        <f>A222&amp;","&amp;B222&amp;"="&amp;C222</f>
-        <v>17,0=0,1</v>
+        <f t="shared" si="3"/>
+        <v>17,0=1,0</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5326,11 +5297,11 @@
       </c>
       <c r="C223" s="1" t="str">
         <f>IF(GraphicMatrix!S3="0","0,1",IF(GraphicMatrix!S3="1","1,0",""))</f>
-        <v>0,1</v>
+        <v>1,0</v>
       </c>
       <c r="D223" s="13" t="str">
-        <f>A223&amp;","&amp;B223&amp;"="&amp;C223</f>
-        <v>17,1=0,1</v>
+        <f t="shared" si="3"/>
+        <v>17,1=1,0</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5345,7 +5316,7 @@
         <v>0,1</v>
       </c>
       <c r="D224" s="13" t="str">
-        <f>A224&amp;","&amp;B224&amp;"="&amp;C224</f>
+        <f t="shared" si="3"/>
         <v>17,2=0,1</v>
       </c>
     </row>
@@ -5361,7 +5332,7 @@
         <v>0,1</v>
       </c>
       <c r="D225" s="13" t="str">
-        <f>A225&amp;","&amp;B225&amp;"="&amp;C225</f>
+        <f t="shared" si="3"/>
         <v>17,3=0,1</v>
       </c>
     </row>
@@ -5377,7 +5348,7 @@
         <v>0,1</v>
       </c>
       <c r="D226" s="13" t="str">
-        <f>A226&amp;","&amp;B226&amp;"="&amp;C226</f>
+        <f t="shared" si="3"/>
         <v>17,4=0,1</v>
       </c>
     </row>
@@ -5393,7 +5364,7 @@
         <v>0,1</v>
       </c>
       <c r="D227" s="13" t="str">
-        <f>A227&amp;","&amp;B227&amp;"="&amp;C227</f>
+        <f t="shared" si="3"/>
         <v>17,5=0,1</v>
       </c>
     </row>
@@ -5409,7 +5380,7 @@
         <v>0,1</v>
       </c>
       <c r="D228" s="13" t="str">
-        <f>A228&amp;","&amp;B228&amp;"="&amp;C228</f>
+        <f t="shared" si="3"/>
         <v>17,6=0,1</v>
       </c>
     </row>
@@ -5425,7 +5396,7 @@
         <v>0,1</v>
       </c>
       <c r="D229" s="13" t="str">
-        <f>A229&amp;","&amp;B229&amp;"="&amp;C229</f>
+        <f t="shared" si="3"/>
         <v>17,7=0,1</v>
       </c>
     </row>
@@ -5441,7 +5412,7 @@
         <v>0,1</v>
       </c>
       <c r="D230" s="13" t="str">
-        <f>A230&amp;","&amp;B230&amp;"="&amp;C230</f>
+        <f t="shared" si="3"/>
         <v>17,8=0,1</v>
       </c>
     </row>
@@ -5457,7 +5428,7 @@
         <v>1,0</v>
       </c>
       <c r="D231" s="13" t="str">
-        <f>A231&amp;","&amp;B231&amp;"="&amp;C231</f>
+        <f t="shared" si="3"/>
         <v>17,9=1,0</v>
       </c>
     </row>
@@ -5473,7 +5444,7 @@
         <v>1,0</v>
       </c>
       <c r="D232" s="13" t="str">
-        <f>A232&amp;","&amp;B232&amp;"="&amp;C232</f>
+        <f t="shared" si="3"/>
         <v>17,10=1,0</v>
       </c>
     </row>
@@ -5489,7 +5460,7 @@
         <v>1,0</v>
       </c>
       <c r="D233" s="13" t="str">
-        <f>A233&amp;","&amp;B233&amp;"="&amp;C233</f>
+        <f t="shared" si="3"/>
         <v>17,11=1,0</v>
       </c>
     </row>
@@ -5505,7 +5476,7 @@
         <v>1,0</v>
       </c>
       <c r="D234" s="13" t="str">
-        <f>A234&amp;","&amp;B234&amp;"="&amp;C234</f>
+        <f t="shared" si="3"/>
         <v>17,12=1,0</v>
       </c>
     </row>
@@ -5521,7 +5492,7 @@
         <v>0,1</v>
       </c>
       <c r="D235" s="13" t="str">
-        <f>A235&amp;","&amp;B235&amp;"="&amp;C235</f>
+        <f t="shared" si="3"/>
         <v>18,0=0,1</v>
       </c>
     </row>
@@ -5537,7 +5508,7 @@
         <v>1,0</v>
       </c>
       <c r="D236" s="13" t="str">
-        <f>A236&amp;","&amp;B236&amp;"="&amp;C236</f>
+        <f t="shared" si="3"/>
         <v>18,1=1,0</v>
       </c>
     </row>
@@ -5553,7 +5524,7 @@
         <v>1,0</v>
       </c>
       <c r="D237" s="13" t="str">
-        <f>A237&amp;","&amp;B237&amp;"="&amp;C237</f>
+        <f t="shared" si="3"/>
         <v>18,2=1,0</v>
       </c>
     </row>
@@ -5569,7 +5540,7 @@
         <v>0,1</v>
       </c>
       <c r="D238" s="13" t="str">
-        <f>A238&amp;","&amp;B238&amp;"="&amp;C238</f>
+        <f t="shared" si="3"/>
         <v>18,3=0,1</v>
       </c>
     </row>
@@ -5585,7 +5556,7 @@
         <v>1,0</v>
       </c>
       <c r="D239" s="13" t="str">
-        <f>A239&amp;","&amp;B239&amp;"="&amp;C239</f>
+        <f t="shared" si="3"/>
         <v>18,4=1,0</v>
       </c>
     </row>
@@ -5601,7 +5572,7 @@
         <v>0,1</v>
       </c>
       <c r="D240" s="13" t="str">
-        <f>A240&amp;","&amp;B240&amp;"="&amp;C240</f>
+        <f t="shared" si="3"/>
         <v>18,5=0,1</v>
       </c>
     </row>
@@ -5617,7 +5588,7 @@
         <v>1,0</v>
       </c>
       <c r="D241" s="13" t="str">
-        <f>A241&amp;","&amp;B241&amp;"="&amp;C241</f>
+        <f t="shared" si="3"/>
         <v>18,6=1,0</v>
       </c>
     </row>
@@ -5633,7 +5604,7 @@
         <v>0,1</v>
       </c>
       <c r="D242" s="13" t="str">
-        <f>A242&amp;","&amp;B242&amp;"="&amp;C242</f>
+        <f t="shared" si="3"/>
         <v>18,7=0,1</v>
       </c>
     </row>
@@ -5649,7 +5620,7 @@
         <v>0,1</v>
       </c>
       <c r="D243" s="13" t="str">
-        <f>A243&amp;","&amp;B243&amp;"="&amp;C243</f>
+        <f t="shared" si="3"/>
         <v>18,8=0,1</v>
       </c>
     </row>
@@ -5665,7 +5636,7 @@
         <v>0,1</v>
       </c>
       <c r="D244" s="13" t="str">
-        <f>A244&amp;","&amp;B244&amp;"="&amp;C244</f>
+        <f t="shared" si="3"/>
         <v>18,9=0,1</v>
       </c>
     </row>
@@ -5681,7 +5652,7 @@
         <v>0,1</v>
       </c>
       <c r="D245" s="13" t="str">
-        <f>A245&amp;","&amp;B245&amp;"="&amp;C245</f>
+        <f t="shared" si="3"/>
         <v>18,10=0,1</v>
       </c>
     </row>
@@ -5697,7 +5668,7 @@
         <v>0,1</v>
       </c>
       <c r="D246" s="13" t="str">
-        <f>A246&amp;","&amp;B246&amp;"="&amp;C246</f>
+        <f t="shared" si="3"/>
         <v>18,11=0,1</v>
       </c>
     </row>
@@ -5713,7 +5684,7 @@
         <v>0,1</v>
       </c>
       <c r="D247" s="13" t="str">
-        <f>A247&amp;","&amp;B247&amp;"="&amp;C247</f>
+        <f t="shared" si="3"/>
         <v>18,12=0,1</v>
       </c>
     </row>
@@ -5729,7 +5700,7 @@
         <v>0,1</v>
       </c>
       <c r="D248" s="13" t="str">
-        <f>A248&amp;","&amp;B248&amp;"="&amp;C248</f>
+        <f t="shared" si="3"/>
         <v>19,0=0,1</v>
       </c>
     </row>
@@ -5745,7 +5716,7 @@
         <v>0,1</v>
       </c>
       <c r="D249" s="13" t="str">
-        <f>A249&amp;","&amp;B249&amp;"="&amp;C249</f>
+        <f t="shared" si="3"/>
         <v>19,1=0,1</v>
       </c>
     </row>
@@ -5761,7 +5732,7 @@
         <v>0,1</v>
       </c>
       <c r="D250" s="13" t="str">
-        <f>A250&amp;","&amp;B250&amp;"="&amp;C250</f>
+        <f t="shared" si="3"/>
         <v>19,2=0,1</v>
       </c>
     </row>
@@ -5777,7 +5748,7 @@
         <v>0,1</v>
       </c>
       <c r="D251" s="13" t="str">
-        <f>A251&amp;","&amp;B251&amp;"="&amp;C251</f>
+        <f t="shared" si="3"/>
         <v>19,3=0,1</v>
       </c>
     </row>
@@ -5793,7 +5764,7 @@
         <v>1,0</v>
       </c>
       <c r="D252" s="13" t="str">
-        <f>A252&amp;","&amp;B252&amp;"="&amp;C252</f>
+        <f t="shared" si="3"/>
         <v>19,4=1,0</v>
       </c>
     </row>
@@ -5809,7 +5780,7 @@
         <v>0,1</v>
       </c>
       <c r="D253" s="13" t="str">
-        <f>A253&amp;","&amp;B253&amp;"="&amp;C253</f>
+        <f t="shared" si="3"/>
         <v>19,5=0,1</v>
       </c>
     </row>
@@ -5825,7 +5796,7 @@
         <v>1,0</v>
       </c>
       <c r="D254" s="13" t="str">
-        <f>A254&amp;","&amp;B254&amp;"="&amp;C254</f>
+        <f t="shared" si="3"/>
         <v>19,6=1,0</v>
       </c>
     </row>
@@ -5841,7 +5812,7 @@
         <v>1,0</v>
       </c>
       <c r="D255" s="13" t="str">
-        <f>A255&amp;","&amp;B255&amp;"="&amp;C255</f>
+        <f t="shared" si="3"/>
         <v>19,7=1,0</v>
       </c>
     </row>
@@ -5857,7 +5828,7 @@
         <v>1,0</v>
       </c>
       <c r="D256" s="13" t="str">
-        <f>A256&amp;","&amp;B256&amp;"="&amp;C256</f>
+        <f t="shared" si="3"/>
         <v>19,8=1,0</v>
       </c>
     </row>
@@ -5873,7 +5844,7 @@
         <v>1,0</v>
       </c>
       <c r="D257" s="13" t="str">
-        <f>A257&amp;","&amp;B257&amp;"="&amp;C257</f>
+        <f t="shared" ref="D257:D312" si="4">A257&amp;","&amp;B257&amp;"="&amp;C257</f>
         <v>19,9=1,0</v>
       </c>
     </row>
@@ -5889,7 +5860,7 @@
         <v>1,0</v>
       </c>
       <c r="D258" s="13" t="str">
-        <f>A258&amp;","&amp;B258&amp;"="&amp;C258</f>
+        <f t="shared" si="4"/>
         <v>19,10=1,0</v>
       </c>
     </row>
@@ -5905,7 +5876,7 @@
         <v>1,0</v>
       </c>
       <c r="D259" s="13" t="str">
-        <f>A259&amp;","&amp;B259&amp;"="&amp;C259</f>
+        <f t="shared" si="4"/>
         <v>19,11=1,0</v>
       </c>
     </row>
@@ -5921,7 +5892,7 @@
         <v>0,1</v>
       </c>
       <c r="D260" s="13" t="str">
-        <f>A260&amp;","&amp;B260&amp;"="&amp;C260</f>
+        <f t="shared" si="4"/>
         <v>19,12=0,1</v>
       </c>
     </row>
@@ -5937,7 +5908,7 @@
         <v>1,0</v>
       </c>
       <c r="D261" s="13" t="str">
-        <f>A261&amp;","&amp;B261&amp;"="&amp;C261</f>
+        <f t="shared" si="4"/>
         <v>20,0=1,0</v>
       </c>
     </row>
@@ -5953,7 +5924,7 @@
         <v>1,0</v>
       </c>
       <c r="D262" s="13" t="str">
-        <f>A262&amp;","&amp;B262&amp;"="&amp;C262</f>
+        <f t="shared" si="4"/>
         <v>20,1=1,0</v>
       </c>
     </row>
@@ -5969,7 +5940,7 @@
         <v>1,0</v>
       </c>
       <c r="D263" s="13" t="str">
-        <f>A263&amp;","&amp;B263&amp;"="&amp;C263</f>
+        <f t="shared" si="4"/>
         <v>20,2=1,0</v>
       </c>
     </row>
@@ -5985,7 +5956,7 @@
         <v>1,0</v>
       </c>
       <c r="D264" s="13" t="str">
-        <f>A264&amp;","&amp;B264&amp;"="&amp;C264</f>
+        <f t="shared" si="4"/>
         <v>20,3=1,0</v>
       </c>
     </row>
@@ -6001,7 +5972,7 @@
         <v>1,0</v>
       </c>
       <c r="D265" s="13" t="str">
-        <f>A265&amp;","&amp;B265&amp;"="&amp;C265</f>
+        <f t="shared" si="4"/>
         <v>20,4=1,0</v>
       </c>
     </row>
@@ -6017,7 +5988,7 @@
         <v>0,1</v>
       </c>
       <c r="D266" s="13" t="str">
-        <f>A266&amp;","&amp;B266&amp;"="&amp;C266</f>
+        <f t="shared" si="4"/>
         <v>20,5=0,1</v>
       </c>
     </row>
@@ -6033,7 +6004,7 @@
         <v>0,1</v>
       </c>
       <c r="D267" s="13" t="str">
-        <f>A267&amp;","&amp;B267&amp;"="&amp;C267</f>
+        <f t="shared" si="4"/>
         <v>20,6=0,1</v>
       </c>
     </row>
@@ -6049,7 +6020,7 @@
         <v>0,1</v>
       </c>
       <c r="D268" s="13" t="str">
-        <f>A268&amp;","&amp;B268&amp;"="&amp;C268</f>
+        <f t="shared" si="4"/>
         <v>20,7=0,1</v>
       </c>
     </row>
@@ -6065,7 +6036,7 @@
         <v>0,1</v>
       </c>
       <c r="D269" s="13" t="str">
-        <f>A269&amp;","&amp;B269&amp;"="&amp;C269</f>
+        <f t="shared" si="4"/>
         <v>20,8=0,1</v>
       </c>
     </row>
@@ -6081,7 +6052,7 @@
         <v>0,1</v>
       </c>
       <c r="D270" s="13" t="str">
-        <f>A270&amp;","&amp;B270&amp;"="&amp;C270</f>
+        <f t="shared" si="4"/>
         <v>20,9=0,1</v>
       </c>
     </row>
@@ -6097,7 +6068,7 @@
         <v>0,1</v>
       </c>
       <c r="D271" s="13" t="str">
-        <f>A271&amp;","&amp;B271&amp;"="&amp;C271</f>
+        <f t="shared" si="4"/>
         <v>20,10=0,1</v>
       </c>
     </row>
@@ -6113,7 +6084,7 @@
         <v>0,1</v>
       </c>
       <c r="D272" s="13" t="str">
-        <f>A272&amp;","&amp;B272&amp;"="&amp;C272</f>
+        <f t="shared" si="4"/>
         <v>20,11=0,1</v>
       </c>
     </row>
@@ -6129,7 +6100,7 @@
         <v>0,1</v>
       </c>
       <c r="D273" s="13" t="str">
-        <f>A273&amp;","&amp;B273&amp;"="&amp;C273</f>
+        <f t="shared" si="4"/>
         <v>20,12=0,1</v>
       </c>
     </row>
@@ -6145,7 +6116,7 @@
         <v>0,1</v>
       </c>
       <c r="D274" s="13" t="str">
-        <f>A274&amp;","&amp;B274&amp;"="&amp;C274</f>
+        <f t="shared" si="4"/>
         <v>21,0=0,1</v>
       </c>
     </row>
@@ -6161,7 +6132,7 @@
         <v>0,1</v>
       </c>
       <c r="D275" s="13" t="str">
-        <f>A275&amp;","&amp;B275&amp;"="&amp;C275</f>
+        <f t="shared" si="4"/>
         <v>21,1=0,1</v>
       </c>
     </row>
@@ -6177,7 +6148,7 @@
         <v>0,1</v>
       </c>
       <c r="D276" s="13" t="str">
-        <f>A276&amp;","&amp;B276&amp;"="&amp;C276</f>
+        <f t="shared" si="4"/>
         <v>21,2=0,1</v>
       </c>
     </row>
@@ -6193,7 +6164,7 @@
         <v>0,1</v>
       </c>
       <c r="D277" s="13" t="str">
-        <f>A277&amp;","&amp;B277&amp;"="&amp;C277</f>
+        <f t="shared" si="4"/>
         <v>21,3=0,1</v>
       </c>
     </row>
@@ -6209,7 +6180,7 @@
         <v>0,1</v>
       </c>
       <c r="D278" s="13" t="str">
-        <f>A278&amp;","&amp;B278&amp;"="&amp;C278</f>
+        <f t="shared" si="4"/>
         <v>21,4=0,1</v>
       </c>
     </row>
@@ -6225,7 +6196,7 @@
         <v>0,1</v>
       </c>
       <c r="D279" s="13" t="str">
-        <f>A279&amp;","&amp;B279&amp;"="&amp;C279</f>
+        <f t="shared" si="4"/>
         <v>21,5=0,1</v>
       </c>
     </row>
@@ -6241,7 +6212,7 @@
         <v>1,0</v>
       </c>
       <c r="D280" s="13" t="str">
-        <f>A280&amp;","&amp;B280&amp;"="&amp;C280</f>
+        <f t="shared" si="4"/>
         <v>21,6=1,0</v>
       </c>
     </row>
@@ -6257,7 +6228,7 @@
         <v>1,0</v>
       </c>
       <c r="D281" s="13" t="str">
-        <f>A281&amp;","&amp;B281&amp;"="&amp;C281</f>
+        <f t="shared" si="4"/>
         <v>21,7=1,0</v>
       </c>
     </row>
@@ -6273,7 +6244,7 @@
         <v>1,0</v>
       </c>
       <c r="D282" s="13" t="str">
-        <f>A282&amp;","&amp;B282&amp;"="&amp;C282</f>
+        <f t="shared" si="4"/>
         <v>21,8=1,0</v>
       </c>
     </row>
@@ -6289,7 +6260,7 @@
         <v>1,0</v>
       </c>
       <c r="D283" s="13" t="str">
-        <f>A283&amp;","&amp;B283&amp;"="&amp;C283</f>
+        <f t="shared" si="4"/>
         <v>21,9=1,0</v>
       </c>
     </row>
@@ -6305,7 +6276,7 @@
         <v>1,0</v>
       </c>
       <c r="D284" s="13" t="str">
-        <f>A284&amp;","&amp;B284&amp;"="&amp;C284</f>
+        <f t="shared" si="4"/>
         <v>21,10=1,0</v>
       </c>
     </row>
@@ -6321,7 +6292,7 @@
         <v>1,0</v>
       </c>
       <c r="D285" s="13" t="str">
-        <f>A285&amp;","&amp;B285&amp;"="&amp;C285</f>
+        <f t="shared" si="4"/>
         <v>21,11=1,0</v>
       </c>
     </row>
@@ -6337,7 +6308,7 @@
         <v>0,1</v>
       </c>
       <c r="D286" s="13" t="str">
-        <f>A286&amp;","&amp;B286&amp;"="&amp;C286</f>
+        <f t="shared" si="4"/>
         <v>21,12=0,1</v>
       </c>
     </row>
@@ -6353,7 +6324,7 @@
         <v>1,0</v>
       </c>
       <c r="D287" s="13" t="str">
-        <f>A287&amp;","&amp;B287&amp;"="&amp;C287</f>
+        <f t="shared" si="4"/>
         <v>22,0=1,0</v>
       </c>
     </row>
@@ -6369,7 +6340,7 @@
         <v>1,0</v>
       </c>
       <c r="D288" s="13" t="str">
-        <f>A288&amp;","&amp;B288&amp;"="&amp;C288</f>
+        <f t="shared" si="4"/>
         <v>22,1=1,0</v>
       </c>
     </row>
@@ -6385,7 +6356,7 @@
         <v>1,0</v>
       </c>
       <c r="D289" s="13" t="str">
-        <f>A289&amp;","&amp;B289&amp;"="&amp;C289</f>
+        <f t="shared" si="4"/>
         <v>22,2=1,0</v>
       </c>
     </row>
@@ -6401,7 +6372,7 @@
         <v>0,1</v>
       </c>
       <c r="D290" s="13" t="str">
-        <f>A290&amp;","&amp;B290&amp;"="&amp;C290</f>
+        <f t="shared" si="4"/>
         <v>22,3=0,1</v>
       </c>
     </row>
@@ -6417,7 +6388,7 @@
         <v>1,0</v>
       </c>
       <c r="D291" s="13" t="str">
-        <f>A291&amp;","&amp;B291&amp;"="&amp;C291</f>
+        <f t="shared" si="4"/>
         <v>22,4=1,0</v>
       </c>
     </row>
@@ -6433,7 +6404,7 @@
         <v>0,1</v>
       </c>
       <c r="D292" s="13" t="str">
-        <f>A292&amp;","&amp;B292&amp;"="&amp;C292</f>
+        <f t="shared" si="4"/>
         <v>22,5=0,1</v>
       </c>
     </row>
@@ -6449,7 +6420,7 @@
         <v>0,1</v>
       </c>
       <c r="D293" s="13" t="str">
-        <f>A293&amp;","&amp;B293&amp;"="&amp;C293</f>
+        <f t="shared" si="4"/>
         <v>22,6=0,1</v>
       </c>
     </row>
@@ -6465,7 +6436,7 @@
         <v>0,1</v>
       </c>
       <c r="D294" s="13" t="str">
-        <f>A294&amp;","&amp;B294&amp;"="&amp;C294</f>
+        <f t="shared" si="4"/>
         <v>22,7=0,1</v>
       </c>
     </row>
@@ -6481,7 +6452,7 @@
         <v>0,1</v>
       </c>
       <c r="D295" s="13" t="str">
-        <f>A295&amp;","&amp;B295&amp;"="&amp;C295</f>
+        <f t="shared" si="4"/>
         <v>22,8=0,1</v>
       </c>
     </row>
@@ -6497,7 +6468,7 @@
         <v>0,1</v>
       </c>
       <c r="D296" s="13" t="str">
-        <f>A296&amp;","&amp;B296&amp;"="&amp;C296</f>
+        <f t="shared" si="4"/>
         <v>22,9=0,1</v>
       </c>
     </row>
@@ -6513,7 +6484,7 @@
         <v>0,1</v>
       </c>
       <c r="D297" s="13" t="str">
-        <f>A297&amp;","&amp;B297&amp;"="&amp;C297</f>
+        <f t="shared" si="4"/>
         <v>22,10=0,1</v>
       </c>
     </row>
@@ -6529,7 +6500,7 @@
         <v>1,0</v>
       </c>
       <c r="D298" s="13" t="str">
-        <f>A298&amp;","&amp;B298&amp;"="&amp;C298</f>
+        <f t="shared" si="4"/>
         <v>22,11=1,0</v>
       </c>
     </row>
@@ -6545,7 +6516,7 @@
         <v>0,1</v>
       </c>
       <c r="D299" s="13" t="str">
-        <f>A299&amp;","&amp;B299&amp;"="&amp;C299</f>
+        <f t="shared" si="4"/>
         <v>22,12=0,1</v>
       </c>
     </row>
@@ -6561,7 +6532,7 @@
         <v>0,1</v>
       </c>
       <c r="D300" s="13" t="str">
-        <f>A300&amp;","&amp;B300&amp;"="&amp;C300</f>
+        <f t="shared" si="4"/>
         <v>23,0=0,1</v>
       </c>
     </row>
@@ -6577,7 +6548,7 @@
         <v>0,1</v>
       </c>
       <c r="D301" s="13" t="str">
-        <f>A301&amp;","&amp;B301&amp;"="&amp;C301</f>
+        <f t="shared" si="4"/>
         <v>23,1=0,1</v>
       </c>
     </row>
@@ -6593,7 +6564,7 @@
         <v>0,1</v>
       </c>
       <c r="D302" s="13" t="str">
-        <f>A302&amp;","&amp;B302&amp;"="&amp;C302</f>
+        <f t="shared" si="4"/>
         <v>23,2=0,1</v>
       </c>
     </row>
@@ -6609,7 +6580,7 @@
         <v>0,1</v>
       </c>
       <c r="D303" s="13" t="str">
-        <f>A303&amp;","&amp;B303&amp;"="&amp;C303</f>
+        <f t="shared" si="4"/>
         <v>23,3=0,1</v>
       </c>
     </row>
@@ -6625,7 +6596,7 @@
         <v>1,0</v>
       </c>
       <c r="D304" s="13" t="str">
-        <f>A304&amp;","&amp;B304&amp;"="&amp;C304</f>
+        <f t="shared" si="4"/>
         <v>23,4=1,0</v>
       </c>
     </row>
@@ -6641,7 +6612,7 @@
         <v>1,0</v>
       </c>
       <c r="D305" s="13" t="str">
-        <f>A305&amp;","&amp;B305&amp;"="&amp;C305</f>
+        <f t="shared" si="4"/>
         <v>23,5=1,0</v>
       </c>
     </row>
@@ -6657,7 +6628,7 @@
         <v>1,0</v>
       </c>
       <c r="D306" s="13" t="str">
-        <f>A306&amp;","&amp;B306&amp;"="&amp;C306</f>
+        <f t="shared" si="4"/>
         <v>23,6=1,0</v>
       </c>
     </row>
@@ -6673,7 +6644,7 @@
         <v>1,0</v>
       </c>
       <c r="D307" s="13" t="str">
-        <f>A307&amp;","&amp;B307&amp;"="&amp;C307</f>
+        <f t="shared" si="4"/>
         <v>23,7=1,0</v>
       </c>
     </row>
@@ -6689,7 +6660,7 @@
         <v>1,0</v>
       </c>
       <c r="D308" s="13" t="str">
-        <f>A308&amp;","&amp;B308&amp;"="&amp;C308</f>
+        <f t="shared" si="4"/>
         <v>23,8=1,0</v>
       </c>
     </row>
@@ -6705,7 +6676,7 @@
         <v>1,0</v>
       </c>
       <c r="D309" s="13" t="str">
-        <f>A309&amp;","&amp;B309&amp;"="&amp;C309</f>
+        <f t="shared" si="4"/>
         <v>23,9=1,0</v>
       </c>
     </row>
@@ -6721,7 +6692,7 @@
         <v>0,1</v>
       </c>
       <c r="D310" s="13" t="str">
-        <f>A310&amp;","&amp;B310&amp;"="&amp;C310</f>
+        <f t="shared" si="4"/>
         <v>23,10=0,1</v>
       </c>
     </row>
@@ -6737,7 +6708,7 @@
         <v>0,1</v>
       </c>
       <c r="D311" s="13" t="str">
-        <f>A311&amp;","&amp;B311&amp;"="&amp;C311</f>
+        <f t="shared" si="4"/>
         <v>23,11=0,1</v>
       </c>
     </row>
@@ -6753,7 +6724,7 @@
         <v>0,1</v>
       </c>
       <c r="D312" s="13" t="str">
-        <f>A312&amp;","&amp;B312&amp;"="&amp;C312</f>
+        <f t="shared" si="4"/>
         <v>23,12=0,1</v>
       </c>
     </row>

</xml_diff>